<commit_message>
Add feature: Security Report Generation
</commit_message>
<xml_diff>
--- a/src/db/database1.xlsx
+++ b/src/db/database1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeril\Documents\SFU\CMPT 782 Cyberlab 1\R&amp;D Project\Project codes\engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SFU\CMPT 782 Cyberlab 1\R&amp;D Project\Project codes\engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D999BD-7454-465B-9AF0-7679B5BC07EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEB0564-DE41-452A-A697-791301D5162E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33555" yWindow="-21675" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="192">
   <si>
     <t>cp /etc/passwd .</t>
   </si>
@@ -726,12 +726,48 @@
   <si>
     <t>ifconfig</t>
   </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sc </t>
+  </si>
+  <si>
+    <t>tftp</t>
+  </si>
+  <si>
+    <t>telnet</t>
+  </si>
+  <si>
+    <t>rundll32</t>
+  </si>
+  <si>
+    <t>LD_PRELOAD</t>
+  </si>
+  <si>
+    <t>5 - Critical</t>
+  </si>
+  <si>
+    <t>4 - High</t>
+  </si>
+  <si>
+    <t>3 - Medium</t>
+  </si>
+  <si>
+    <t>2 - Low</t>
+  </si>
+  <si>
+    <t>1 - Informational</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,6 +834,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -819,7 +862,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -883,11 +926,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -928,12 +984,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,643 +1276,761 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="135.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="132.77734375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="B15" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7">
-        <v>3</v>
+      <c r="B16" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7">
-        <v>4</v>
+      <c r="B17" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7">
-        <v>4</v>
+      <c r="B18" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7">
-        <v>4</v>
+      <c r="B19" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="7">
-        <v>4</v>
+      <c r="B20" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="7">
-        <v>4</v>
+      <c r="B21" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="7">
-        <v>4</v>
+      <c r="B22" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="7">
-        <v>4</v>
+      <c r="B23" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="B47" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="B48" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="B49" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="B50" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="B51" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="B52" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="B53" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="B54" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="B55" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="B56" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
+      <c r="B57" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
+      <c r="B58" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B52" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B54" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B55" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B57" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="14" t="s">
+      <c r="B59" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="B58" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="14" t="s">
+      <c r="B60" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B60" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="15" t="s">
+      <c r="B61" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B61" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="15" t="s">
+      <c r="B62" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B62" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B63" s="7">
-        <v>4</v>
+      <c r="B63" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="B64" s="7">
-        <v>4</v>
+      <c r="A64" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" s="7">
-        <v>4</v>
+      <c r="A65" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B66" s="7">
-        <v>4</v>
+      <c r="A66" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B67" s="7">
-        <v>5</v>
+      <c r="A67" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B68" s="7">
-        <v>3</v>
+        <v>173</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" s="7">
-        <v>3</v>
+      <c r="A69" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B70" s="7">
-        <v>3</v>
+        <v>111</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B71" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="17" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B72" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" s="17" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="B73" s="7">
-        <v>3</v>
+        <v>182</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B74" s="7">
-        <v>3</v>
+        <v>130</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" s="7">
-        <v>2</v>
+        <v>140</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B76" s="7">
-        <v>2</v>
+      <c r="A76" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B77" s="7">
-        <v>2</v>
+      <c r="A77" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="7">
-        <v>3</v>
-      </c>
+      <c r="B89" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="22"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B92">
+    <sortCondition descending="1" ref="B44:B92"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2041,13 +2221,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="20" t="s">
         <v>120</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -2055,11 +2235,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="16" t="s">
         <v>122</v>
       </c>
@@ -2163,48 +2343,48 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="20" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>152</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="20" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">

</xml_diff>